<commit_message>
CreatePriceList test case added
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,27 +4,44 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000"/>
+    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateNewLead" sheetId="1" r:id="rId1"/>
+    <sheet name="CreatePriceList" sheetId="2" r:id="rId2"/>
+    <sheet name="CreatePriceListItems" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+  <si>
+    <t>2/1/2020</t>
+  </si>
+  <si>
+    <t>ArmBand 100</t>
+  </si>
   <si>
     <t>JobTitle</t>
   </si>
   <si>
+    <t>EndDate</t>
+  </si>
+  <si>
     <t>LeadSource</t>
   </si>
   <si>
+    <t>2/1/2030</t>
+  </si>
+  <si>
     <t>MyTopic</t>
   </si>
   <si>
+    <t>ArmBand 150</t>
+  </si>
+  <si>
     <t>Hot</t>
   </si>
   <si>
@@ -34,13 +51,40 @@
     <t>John</t>
   </si>
   <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>TestPriceList</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Rating</t>
   </si>
   <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Price list for testing purposes</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
+    <t>Basic Package</t>
+  </si>
+  <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>CEO</t>
@@ -93,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +443,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection activeCell="$F$3" sqref="$F$3:$F$3"/>
     </sheetView>
   </sheetViews>
@@ -411,43 +458,158 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$C$3" sqref="$C$3:$C$3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$C$4" sqref="$C$4:$C$4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.99609375" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>